<commit_message>
Added additional column in read data from excel file.
</commit_message>
<xml_diff>
--- a/src/test/resources/dataSources/LoginTest.xlsx
+++ b/src/test/resources/dataSources/LoginTest.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="42">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -54,12 +54,6 @@
     <t>openBrowser</t>
   </si>
   <si>
-    <t>enterUserName</t>
-  </si>
-  <si>
-    <t>enterPassword</t>
-  </si>
-  <si>
     <t>Click on login button</t>
   </si>
   <si>
@@ -129,13 +123,25 @@
     <t>Result</t>
   </si>
   <si>
-    <t>ClickLogin</t>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>german</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Arabic</t>
+  </si>
+  <si>
+    <t>http://demo.silverstripe.org/Security/login</t>
+  </si>
+  <si>
+    <t>enterText</t>
   </si>
   <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -143,7 +149,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +164,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -192,17 +205,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -511,13 +530,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -525,27 +544,27 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -555,10 +574,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -567,9 +586,10 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
     <col min="3" max="4" customWidth="true" width="39.0" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="41.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -580,16 +600,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -603,16 +626,17 @@
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="F2" s="2"/>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
@@ -621,113 +645,134 @@
       <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="F3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>40</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>40</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>33</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F8" s="2"/>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -736,9 +781,10 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="40.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -749,18 +795,21 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -772,16 +821,17 @@
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="F2" s="2"/>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
@@ -790,107 +840,122 @@
       <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="F3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>14</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" t="s">
-        <v>38</v>
+        <v>16</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>